<commit_message>
corrección de escaletas CN_07_11_CO; CN_07_12_CO; CN_08_11_CO; CN_08_12_CO;
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado07/guion11/Escaleta_CN_07_11_CO.xlsx
+++ b/fuentes/contenidos/grado07/guion11/Escaleta_CN_07_11_CO.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\psf\Home\Documents\Aula Planeta Colombia\Repositorios\CienciasNaturales\fuentes\contenidos\grado07\guion11\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\MIS DOCUMENTOS\Desktop\CienciasNaturales\fuentes\contenidos\grado07\guion11\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="121" windowWidth="19444" windowHeight="8926"/>
+    <workbookView xWindow="0" yWindow="120" windowWidth="19440" windowHeight="8925"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja2" sheetId="2" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="658" uniqueCount="277">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="662" uniqueCount="275">
   <si>
     <t>Asignatura</t>
   </si>
@@ -515,9 +515,6 @@
     <t xml:space="preserve">Actividad que permite estudiar los conceptos de fuerzas eléctricas y magnéticas </t>
   </si>
   <si>
-    <t>Refuerza tu aprendizaje: practica lo que aprendiste sobre fuerzas</t>
-  </si>
-  <si>
     <t>Refuerza tu aprendizaje: Las fuerzas fundamentales</t>
   </si>
   <si>
@@ -680,18 +677,12 @@
     <t>Competencias</t>
   </si>
   <si>
-    <t>Competencias: Estudio de las fuerzas y sus características</t>
-  </si>
-  <si>
     <t>Actividad que propone un experimento para realizar una representación gráfica de cómo actúan las fuerzas</t>
   </si>
   <si>
     <t>Competencias: estudio de las fuerzas y sus características</t>
   </si>
   <si>
-    <t>Competencias: Comprobación del principio de Arquímedes</t>
-  </si>
-  <si>
     <t>Actividad que propone un experimento para comprobar cómo funciona de forma práctica el principio de Arquímedes</t>
   </si>
   <si>
@@ -710,9 +701,6 @@
     <t>FQ_10_02</t>
   </si>
   <si>
-    <t>Competencias: Comprueba tus conocimientos sobre las fuerzas en equilibrio</t>
-  </si>
-  <si>
     <t>Competencias: equilibrio de fuerzas</t>
   </si>
   <si>
@@ -734,9 +722,6 @@
     <t xml:space="preserve">Actividad que propone desarrollar ejercicios relacionados con la fórmula de trabajo </t>
   </si>
   <si>
-    <t>Refuerza tu aprendizaje: los sistemas en equilibrio</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Comprueba tus conocimientos sobre las fuerzas</t>
   </si>
   <si>
@@ -746,19 +731,10 @@
     <t>Actividad para ejercitar la relación de los conceptos de fuerza con sus definiciones</t>
   </si>
   <si>
-    <t>CN_06_09_CO</t>
-  </si>
-  <si>
     <t>La materia y sus propiedades</t>
   </si>
   <si>
     <t>Fin de unidad</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Banco de actividades: La materia y sus propiedades </t>
-  </si>
-  <si>
-    <t>Motor que incluye preguntas de respuesta abierta del tema La materia y  sus propiedades</t>
   </si>
   <si>
     <t>Mapa Conceptual</t>
@@ -862,6 +838,24 @@
   </si>
   <si>
     <t>Evalúa tus conocimientos sobre el tema Las fuerzas y sus efectos sobre los objetos</t>
+  </si>
+  <si>
+    <t>Refuerza tu aprendizaje: Practica lo que aprendiste sobre fuerzas</t>
+  </si>
+  <si>
+    <t>Refuerza tu aprendizaje: Los sistemas en equilibrio</t>
+  </si>
+  <si>
+    <t>Competencias: comprueba tus conocimientos sobre las fuerzas en equilibrio</t>
+  </si>
+  <si>
+    <t>Motor que incluye preguntas de respuesta abierta del tema Las fuerzas y sus efectos sobre los objetos</t>
+  </si>
+  <si>
+    <t>Banco de actividades: Las fuerzas y sus efectos sobre los objetos</t>
+  </si>
+  <si>
+    <t>Recurso M101AP-01</t>
   </si>
 </sst>
 </file>
@@ -1717,36 +1711,36 @@
   <sheetPr codeName="Hoja2"/>
   <dimension ref="A1:U123"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M33" sqref="M33"/>
+    <sheetView tabSelected="1" topLeftCell="G14" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Q34" sqref="Q34:U34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.86328125" customWidth="1"/>
-    <col min="2" max="2" width="17.59765625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.3984375" customWidth="1"/>
-    <col min="4" max="4" width="34.1328125" customWidth="1"/>
-    <col min="5" max="5" width="32.86328125" customWidth="1"/>
-    <col min="6" max="6" width="32.86328125" style="22" customWidth="1"/>
-    <col min="7" max="7" width="36.59765625" customWidth="1"/>
-    <col min="8" max="8" width="10.73046875" style="22" customWidth="1"/>
-    <col min="9" max="9" width="8.73046875" style="22" customWidth="1"/>
-    <col min="10" max="10" width="30.265625" customWidth="1"/>
+    <col min="1" max="1" width="15.85546875" customWidth="1"/>
+    <col min="2" max="2" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.42578125" customWidth="1"/>
+    <col min="4" max="4" width="34.140625" customWidth="1"/>
+    <col min="5" max="5" width="32.85546875" customWidth="1"/>
+    <col min="6" max="6" width="32.85546875" style="22" customWidth="1"/>
+    <col min="7" max="7" width="36.5703125" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" style="22" customWidth="1"/>
+    <col min="9" max="9" width="8.7109375" style="22" customWidth="1"/>
+    <col min="10" max="10" width="30.28515625" customWidth="1"/>
     <col min="11" max="11" width="14" customWidth="1"/>
-    <col min="12" max="12" width="17.73046875" customWidth="1"/>
-    <col min="13" max="13" width="13.86328125" customWidth="1"/>
-    <col min="14" max="14" width="15.59765625" customWidth="1"/>
-    <col min="15" max="15" width="29.265625" style="22" customWidth="1"/>
-    <col min="16" max="16" width="21.59765625" style="22" customWidth="1"/>
-    <col min="17" max="17" width="16.1328125" style="22" customWidth="1"/>
-    <col min="18" max="18" width="16.59765625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="14.73046875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="18.265625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.7109375" customWidth="1"/>
+    <col min="13" max="13" width="13.85546875" customWidth="1"/>
+    <col min="14" max="14" width="15.5703125" customWidth="1"/>
+    <col min="15" max="15" width="29.28515625" style="22" customWidth="1"/>
+    <col min="16" max="16" width="21.5703125" style="22" customWidth="1"/>
+    <col min="17" max="17" width="16.140625" style="22" customWidth="1"/>
+    <col min="18" max="18" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18.28515625" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="33.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:21" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="84" t="s">
         <v>0</v>
       </c>
@@ -1809,7 +1803,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="2" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="84"/>
       <c r="B2" s="83"/>
       <c r="C2" s="91"/>
@@ -1836,7 +1830,7 @@
       <c r="T2" s="94"/>
       <c r="U2" s="93"/>
     </row>
-    <row r="3" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>122</v>
       </c>
@@ -1861,7 +1855,7 @@
         <v>126</v>
       </c>
       <c r="J3" s="27" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
       <c r="K3" s="13" t="s">
         <v>19</v>
@@ -1874,7 +1868,7 @@
       </c>
       <c r="N3" s="28"/>
       <c r="O3" s="29" t="s">
-        <v>263</v>
+        <v>255</v>
       </c>
       <c r="P3" s="29" t="s">
         <v>19</v>
@@ -1895,7 +1889,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="4" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>122</v>
       </c>
@@ -1924,7 +1918,7 @@
         <v>135</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="K4" s="13" t="s">
         <v>20</v>
@@ -1937,7 +1931,7 @@
         <v>32</v>
       </c>
       <c r="O4" s="20" t="s">
-        <v>264</v>
+        <v>256</v>
       </c>
       <c r="P4" s="21" t="s">
         <v>19</v>
@@ -1958,7 +1952,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="5" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>122</v>
       </c>
@@ -1998,7 +1992,7 @@
       <c r="M5" s="14"/>
       <c r="N5" s="14"/>
       <c r="O5" s="20" t="s">
-        <v>263</v>
+        <v>255</v>
       </c>
       <c r="P5" s="21" t="s">
         <v>19</v>
@@ -2019,7 +2013,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="6" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>122</v>
       </c>
@@ -2048,7 +2042,7 @@
         <v>135</v>
       </c>
       <c r="J6" s="5" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="K6" s="13" t="s">
         <v>20</v>
@@ -2061,7 +2055,7 @@
         <v>23</v>
       </c>
       <c r="O6" s="20" t="s">
-        <v>265</v>
+        <v>257</v>
       </c>
       <c r="P6" s="21" t="s">
         <v>20</v>
@@ -2082,7 +2076,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="7" spans="1:21" s="53" customFormat="1" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:21" s="53" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="38" t="s">
         <v>122</v>
       </c>
@@ -2100,7 +2094,7 @@
       </c>
       <c r="F7" s="42"/>
       <c r="G7" s="43" t="s">
-        <v>163</v>
+        <v>269</v>
       </c>
       <c r="H7" s="76">
         <v>5</v>
@@ -2122,7 +2116,7 @@
         <v>52</v>
       </c>
       <c r="O7" s="42" t="s">
-        <v>266</v>
+        <v>258</v>
       </c>
       <c r="P7" s="49" t="s">
         <v>19</v>
@@ -2143,7 +2137,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="8" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>122</v>
       </c>
@@ -2168,7 +2162,7 @@
         <v>126</v>
       </c>
       <c r="J8" s="37" t="s">
-        <v>247</v>
+        <v>239</v>
       </c>
       <c r="K8" s="13" t="s">
         <v>20</v>
@@ -2181,7 +2175,7 @@
       </c>
       <c r="N8" s="14"/>
       <c r="O8" s="21" t="s">
-        <v>264</v>
+        <v>256</v>
       </c>
       <c r="P8" s="21" t="s">
         <v>19</v>
@@ -2190,19 +2184,19 @@
         <v>6</v>
       </c>
       <c r="R8" s="15" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
       <c r="S8" s="16" t="s">
-        <v>249</v>
+        <v>241</v>
       </c>
       <c r="T8" s="17" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="U8" s="16" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="9" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>122</v>
       </c>
@@ -2240,7 +2234,7 @@
       <c r="M9" s="14"/>
       <c r="N9" s="14"/>
       <c r="O9" s="79" t="s">
-        <v>267</v>
+        <v>259</v>
       </c>
       <c r="P9" s="21" t="s">
         <v>19</v>
@@ -2261,7 +2255,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="10" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>122</v>
       </c>
@@ -2301,7 +2295,7 @@
         <v>101</v>
       </c>
       <c r="O10" s="20" t="s">
-        <v>264</v>
+        <v>256</v>
       </c>
       <c r="P10" s="21" t="s">
         <v>19</v>
@@ -2322,7 +2316,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="11" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
         <v>122</v>
       </c>
@@ -2349,7 +2343,7 @@
         <v>135</v>
       </c>
       <c r="J11" s="5" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="K11" s="13" t="s">
         <v>20</v>
@@ -2362,7 +2356,7 @@
         <v>95</v>
       </c>
       <c r="O11" s="20" t="s">
-        <v>264</v>
+        <v>256</v>
       </c>
       <c r="P11" s="21" t="s">
         <v>19</v>
@@ -2383,7 +2377,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="12" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>122</v>
       </c>
@@ -2401,7 +2395,7 @@
       </c>
       <c r="F12" s="20"/>
       <c r="G12" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="H12" s="33">
         <v>10</v>
@@ -2410,7 +2404,7 @@
         <v>135</v>
       </c>
       <c r="J12" s="5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="K12" s="13" t="s">
         <v>20</v>
@@ -2423,7 +2417,7 @@
         <v>52</v>
       </c>
       <c r="O12" s="70" t="s">
-        <v>264</v>
+        <v>256</v>
       </c>
       <c r="P12" s="21" t="s">
         <v>19</v>
@@ -2438,13 +2432,13 @@
         <v>138</v>
       </c>
       <c r="T12" s="8" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="U12" s="7" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="13" spans="1:21" s="53" customFormat="1" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:21" s="53" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="38" t="s">
         <v>122</v>
       </c>
@@ -2462,7 +2456,7 @@
       </c>
       <c r="F13" s="42"/>
       <c r="G13" s="43" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="H13" s="33">
         <v>11</v>
@@ -2471,7 +2465,7 @@
         <v>135</v>
       </c>
       <c r="J13" s="45" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="K13" s="46" t="s">
         <v>20</v>
@@ -2484,7 +2478,7 @@
         <v>33</v>
       </c>
       <c r="O13" s="42" t="s">
-        <v>264</v>
+        <v>256</v>
       </c>
       <c r="P13" s="42" t="s">
         <v>20</v>
@@ -2499,13 +2493,13 @@
         <v>138</v>
       </c>
       <c r="T13" s="52" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
       <c r="U13" s="50" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="14" spans="1:21" s="64" customFormat="1" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:21" s="64" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
         <v>122</v>
       </c>
@@ -2516,7 +2510,7 @@
         <v>124</v>
       </c>
       <c r="D14" s="34" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E14" s="75"/>
       <c r="F14" s="55"/>
@@ -2530,7 +2524,7 @@
         <v>126</v>
       </c>
       <c r="J14" s="57" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="K14" s="58" t="s">
         <v>20</v>
@@ -2543,7 +2537,7 @@
       </c>
       <c r="N14" s="60"/>
       <c r="O14" s="55" t="s">
-        <v>268</v>
+        <v>260</v>
       </c>
       <c r="P14" s="21" t="s">
         <v>19</v>
@@ -2555,16 +2549,16 @@
         <v>137</v>
       </c>
       <c r="S14" s="61" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="T14" s="63" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="U14" s="61" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="15" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
         <v>122</v>
       </c>
@@ -2575,14 +2569,14 @@
         <v>124</v>
       </c>
       <c r="D15" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="E15" s="35" t="s">
         <v>169</v>
-      </c>
-      <c r="E15" s="35" t="s">
-        <v>170</v>
       </c>
       <c r="F15" s="20"/>
       <c r="G15" s="4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="H15" s="33">
         <v>13</v>
@@ -2591,7 +2585,7 @@
         <v>126</v>
       </c>
       <c r="J15" s="5" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="K15" s="13" t="s">
         <v>19</v>
@@ -2602,7 +2596,7 @@
       <c r="M15" s="14"/>
       <c r="N15" s="14"/>
       <c r="O15" s="79" t="s">
-        <v>269</v>
+        <v>261</v>
       </c>
       <c r="P15" s="21" t="s">
         <v>19</v>
@@ -2611,19 +2605,19 @@
         <v>143</v>
       </c>
       <c r="R15" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="S15" s="7" t="s">
         <v>194</v>
       </c>
-      <c r="S15" s="7" t="s">
+      <c r="T15" s="8" t="s">
         <v>195</v>
       </c>
-      <c r="T15" s="8" t="s">
+      <c r="U15" s="7" t="s">
         <v>196</v>
       </c>
-      <c r="U15" s="7" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="16" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
+    </row>
+    <row r="16" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
         <v>122</v>
       </c>
@@ -2634,16 +2628,16 @@
         <v>124</v>
       </c>
       <c r="D16" s="34" t="s">
+        <v>168</v>
+      </c>
+      <c r="E16" s="35" t="s">
         <v>169</v>
       </c>
-      <c r="E16" s="35" t="s">
+      <c r="F16" s="21" t="s">
         <v>170</v>
       </c>
-      <c r="F16" s="21" t="s">
-        <v>171</v>
-      </c>
       <c r="G16" s="36" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="H16" s="33">
         <v>14</v>
@@ -2652,7 +2646,7 @@
         <v>135</v>
       </c>
       <c r="J16" s="37" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="K16" s="13" t="s">
         <v>19</v>
@@ -2663,28 +2657,28 @@
       <c r="M16" s="14"/>
       <c r="N16" s="14"/>
       <c r="O16" s="21" t="s">
-        <v>266</v>
+        <v>258</v>
       </c>
       <c r="P16" s="21" t="s">
         <v>19</v>
       </c>
       <c r="Q16" s="16" t="s">
+        <v>172</v>
+      </c>
+      <c r="R16" s="15" t="s">
         <v>173</v>
       </c>
-      <c r="R16" s="15" t="s">
+      <c r="S16" s="16" t="s">
         <v>174</v>
       </c>
-      <c r="S16" s="16" t="s">
+      <c r="T16" s="17" t="s">
         <v>175</v>
       </c>
-      <c r="T16" s="17" t="s">
+      <c r="U16" s="16" t="s">
         <v>176</v>
       </c>
-      <c r="U16" s="16" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="17" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
+    </row>
+    <row r="17" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
         <v>122</v>
       </c>
@@ -2695,16 +2689,16 @@
         <v>124</v>
       </c>
       <c r="D17" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="E17" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="E17" s="2" t="s">
-        <v>170</v>
-      </c>
       <c r="F17" s="20" t="s">
+        <v>177</v>
+      </c>
+      <c r="G17" s="4" t="s">
         <v>178</v>
-      </c>
-      <c r="G17" s="4" t="s">
-        <v>179</v>
       </c>
       <c r="H17" s="33">
         <v>15</v>
@@ -2713,7 +2707,7 @@
         <v>126</v>
       </c>
       <c r="J17" s="5" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="K17" s="13" t="s">
         <v>19</v>
@@ -2724,7 +2718,7 @@
       <c r="M17" s="14"/>
       <c r="N17" s="14"/>
       <c r="O17" s="20" t="s">
-        <v>263</v>
+        <v>255</v>
       </c>
       <c r="P17" s="21" t="s">
         <v>19</v>
@@ -2739,13 +2733,13 @@
         <v>129</v>
       </c>
       <c r="T17" s="8" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="U17" s="7" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="18" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
         <v>122</v>
       </c>
@@ -2756,16 +2750,16 @@
         <v>124</v>
       </c>
       <c r="D18" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="E18" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="E18" s="2" t="s">
-        <v>170</v>
-      </c>
       <c r="F18" s="20" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="H18" s="33">
         <v>16</v>
@@ -2774,7 +2768,7 @@
         <v>135</v>
       </c>
       <c r="J18" s="5" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="K18" s="13" t="s">
         <v>19</v>
@@ -2785,7 +2779,7 @@
       <c r="M18" s="14"/>
       <c r="N18" s="14"/>
       <c r="O18" s="20" t="s">
-        <v>270</v>
+        <v>262</v>
       </c>
       <c r="P18" s="21" t="s">
         <v>19</v>
@@ -2800,13 +2794,13 @@
         <v>129</v>
       </c>
       <c r="T18" s="8" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="U18" s="7" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="19" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
         <v>122</v>
       </c>
@@ -2817,14 +2811,14 @@
         <v>124</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="F19" s="20"/>
       <c r="G19" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="H19" s="33">
         <v>17</v>
@@ -2833,7 +2827,7 @@
         <v>126</v>
       </c>
       <c r="J19" s="5" t="s">
-        <v>259</v>
+        <v>251</v>
       </c>
       <c r="K19" s="13" t="s">
         <v>20</v>
@@ -2846,7 +2840,7 @@
       </c>
       <c r="N19" s="14"/>
       <c r="O19" s="20" t="s">
-        <v>271</v>
+        <v>263</v>
       </c>
       <c r="P19" s="21" t="s">
         <v>19</v>
@@ -2855,19 +2849,19 @@
         <v>6</v>
       </c>
       <c r="R19" s="6" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
       <c r="S19" s="7" t="s">
-        <v>249</v>
+        <v>241</v>
       </c>
       <c r="T19" s="8" t="s">
-        <v>260</v>
+        <v>252</v>
       </c>
       <c r="U19" s="7" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="20" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
         <v>122</v>
       </c>
@@ -2878,16 +2872,16 @@
         <v>124</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="F20" s="20" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="H20" s="33">
         <v>18</v>
@@ -2896,7 +2890,7 @@
         <v>126</v>
       </c>
       <c r="J20" s="5" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="K20" s="13" t="s">
         <v>19</v>
@@ -2907,7 +2901,7 @@
       <c r="M20" s="14"/>
       <c r="N20" s="14"/>
       <c r="O20" s="20" t="s">
-        <v>263</v>
+        <v>255</v>
       </c>
       <c r="P20" s="21" t="s">
         <v>19</v>
@@ -2922,13 +2916,13 @@
         <v>129</v>
       </c>
       <c r="T20" s="8" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="U20" s="7" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="21" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="21" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
         <v>122</v>
       </c>
@@ -2939,16 +2933,16 @@
         <v>124</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E21" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="F21" s="20" t="s">
         <v>184</v>
       </c>
-      <c r="F21" s="20" t="s">
+      <c r="G21" s="4" t="s">
         <v>185</v>
-      </c>
-      <c r="G21" s="4" t="s">
-        <v>186</v>
       </c>
       <c r="H21" s="33">
         <v>19</v>
@@ -2957,7 +2951,7 @@
         <v>126</v>
       </c>
       <c r="J21" s="5" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="K21" s="13" t="s">
         <v>19</v>
@@ -2968,7 +2962,7 @@
       <c r="M21" s="14"/>
       <c r="N21" s="14"/>
       <c r="O21" s="20" t="s">
-        <v>263</v>
+        <v>255</v>
       </c>
       <c r="P21" s="21" t="s">
         <v>19</v>
@@ -2977,19 +2971,19 @@
         <v>5</v>
       </c>
       <c r="R21" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="S21" s="7" t="s">
         <v>188</v>
       </c>
-      <c r="S21" s="7" t="s">
+      <c r="T21" s="8" t="s">
         <v>189</v>
       </c>
-      <c r="T21" s="8" t="s">
+      <c r="U21" s="7" t="s">
         <v>190</v>
       </c>
-      <c r="U21" s="7" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="22" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
+    </row>
+    <row r="22" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
         <v>122</v>
       </c>
@@ -3000,14 +2994,14 @@
         <v>124</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E22" s="2" t="s">
         <v>147</v>
       </c>
       <c r="F22" s="20"/>
       <c r="G22" s="4" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="H22" s="33">
         <v>20</v>
@@ -3016,7 +3010,7 @@
         <v>135</v>
       </c>
       <c r="J22" s="5" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="K22" s="13" t="s">
         <v>20</v>
@@ -3029,7 +3023,7 @@
         <v>52</v>
       </c>
       <c r="O22" s="20" t="s">
-        <v>264</v>
+        <v>256</v>
       </c>
       <c r="P22" s="21" t="s">
         <v>19</v>
@@ -3044,13 +3038,13 @@
         <v>138</v>
       </c>
       <c r="T22" s="8" t="s">
-        <v>261</v>
+        <v>253</v>
       </c>
       <c r="U22" s="7" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="23" spans="1:21" s="53" customFormat="1" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="23" spans="1:21" s="53" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="38" t="s">
         <v>122</v>
       </c>
@@ -3061,14 +3055,14 @@
         <v>124</v>
       </c>
       <c r="D23" s="65" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E23" s="41" t="s">
         <v>147</v>
       </c>
       <c r="F23" s="42"/>
       <c r="G23" s="43" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="H23" s="78">
         <v>21</v>
@@ -3077,7 +3071,7 @@
         <v>135</v>
       </c>
       <c r="J23" s="45" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="K23" s="46" t="s">
         <v>20</v>
@@ -3090,7 +3084,7 @@
         <v>33</v>
       </c>
       <c r="O23" s="42" t="s">
-        <v>264</v>
+        <v>256</v>
       </c>
       <c r="P23" s="49" t="s">
         <v>20</v>
@@ -3105,13 +3099,13 @@
         <v>138</v>
       </c>
       <c r="T23" s="52" t="s">
-        <v>262</v>
+        <v>254</v>
       </c>
       <c r="U23" s="50" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="24" spans="1:21" s="77" customFormat="1" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="24" spans="1:21" s="77" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
         <v>122</v>
       </c>
@@ -3122,12 +3116,12 @@
         <v>124</v>
       </c>
       <c r="D24" s="34" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E24" s="35"/>
       <c r="F24" s="21"/>
       <c r="G24" s="36" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="H24" s="33">
         <v>22</v>
@@ -3136,7 +3130,7 @@
         <v>126</v>
       </c>
       <c r="J24" s="37" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="K24" s="13" t="s">
         <v>19</v>
@@ -3147,28 +3141,28 @@
       <c r="M24" s="14"/>
       <c r="N24" s="14"/>
       <c r="O24" s="21" t="s">
-        <v>263</v>
+        <v>255</v>
       </c>
       <c r="P24" s="21" t="s">
         <v>19</v>
       </c>
       <c r="Q24" s="16" t="s">
+        <v>172</v>
+      </c>
+      <c r="R24" s="15" t="s">
         <v>173</v>
       </c>
-      <c r="R24" s="15" t="s">
+      <c r="S24" s="16" t="s">
         <v>174</v>
       </c>
-      <c r="S24" s="16" t="s">
-        <v>175</v>
-      </c>
       <c r="T24" s="17" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="U24" s="16" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="25" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
         <v>122</v>
       </c>
@@ -3179,14 +3173,14 @@
         <v>124</v>
       </c>
       <c r="D25" s="34" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E25" s="35" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="F25" s="21"/>
       <c r="G25" s="36" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="H25" s="33">
         <v>23</v>
@@ -3195,7 +3189,7 @@
         <v>135</v>
       </c>
       <c r="J25" s="37" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="K25" s="13" t="s">
         <v>20</v>
@@ -3208,7 +3202,7 @@
         <v>32</v>
       </c>
       <c r="O25" s="21" t="s">
-        <v>271</v>
+        <v>263</v>
       </c>
       <c r="P25" s="21" t="s">
         <v>19</v>
@@ -3223,13 +3217,13 @@
         <v>138</v>
       </c>
       <c r="T25" s="17" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="U25" s="16" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="26" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="26" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
         <v>122</v>
       </c>
@@ -3240,14 +3234,14 @@
         <v>124</v>
       </c>
       <c r="D26" s="34" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F26" s="20"/>
       <c r="G26" s="4" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="H26" s="33">
         <v>24</v>
@@ -3256,7 +3250,7 @@
         <v>135</v>
       </c>
       <c r="J26" s="5" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="K26" s="66" t="s">
         <v>20</v>
@@ -3269,7 +3263,7 @@
         <v>104</v>
       </c>
       <c r="O26" s="20" t="s">
-        <v>271</v>
+        <v>263</v>
       </c>
       <c r="P26" s="21" t="s">
         <v>19</v>
@@ -3284,13 +3278,13 @@
         <v>138</v>
       </c>
       <c r="T26" s="8" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="U26" s="7" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="27" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="27" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="9" t="s">
         <v>122</v>
       </c>
@@ -3301,14 +3295,14 @@
         <v>124</v>
       </c>
       <c r="D27" s="34" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F27" s="20"/>
       <c r="G27" s="4" t="s">
-        <v>236</v>
+        <v>270</v>
       </c>
       <c r="H27" s="33">
         <v>25</v>
@@ -3317,7 +3311,7 @@
         <v>135</v>
       </c>
       <c r="J27" s="5" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="K27" s="66" t="s">
         <v>19</v>
@@ -3330,7 +3324,7 @@
         <v>52</v>
       </c>
       <c r="O27" s="20" t="s">
-        <v>266</v>
+        <v>258</v>
       </c>
       <c r="P27" s="21" t="s">
         <v>19</v>
@@ -3345,13 +3339,13 @@
         <v>129</v>
       </c>
       <c r="T27" s="8" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="U27" s="7" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="28" spans="1:21" s="53" customFormat="1" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="28" spans="1:21" s="53" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="38" t="s">
         <v>122</v>
       </c>
@@ -3362,14 +3356,14 @@
         <v>124</v>
       </c>
       <c r="D28" s="54" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E28" s="41" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F28" s="42"/>
       <c r="G28" s="43" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="H28" s="33">
         <v>26</v>
@@ -3378,7 +3372,7 @@
         <v>135</v>
       </c>
       <c r="J28" s="45" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="K28" s="72" t="s">
         <v>19</v>
@@ -3389,28 +3383,28 @@
       <c r="M28" s="74"/>
       <c r="N28" s="48"/>
       <c r="O28" s="42" t="s">
-        <v>272</v>
+        <v>264</v>
       </c>
       <c r="P28" s="49" t="s">
         <v>20</v>
       </c>
       <c r="Q28" s="50" t="s">
+        <v>172</v>
+      </c>
+      <c r="R28" s="51" t="s">
         <v>173</v>
       </c>
-      <c r="R28" s="51" t="s">
-        <v>174</v>
-      </c>
       <c r="S28" s="50" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="T28" s="52" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="U28" s="50" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="29" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="9" t="s">
         <v>122</v>
       </c>
@@ -3421,7 +3415,7 @@
         <v>124</v>
       </c>
       <c r="D29" s="34" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E29" s="35"/>
       <c r="F29" s="21"/>
@@ -3435,7 +3429,7 @@
         <v>135</v>
       </c>
       <c r="J29" s="37" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="K29" s="66" t="s">
         <v>19</v>
@@ -3445,10 +3439,10 @@
       </c>
       <c r="M29" s="67"/>
       <c r="N29" s="14" t="s">
-        <v>275</v>
+        <v>267</v>
       </c>
       <c r="O29" s="21" t="s">
-        <v>266</v>
+        <v>258</v>
       </c>
       <c r="P29" s="21" t="s">
         <v>19</v>
@@ -3463,13 +3457,13 @@
         <v>129</v>
       </c>
       <c r="T29" s="17" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="U29" s="16" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="30" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="30" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="9" t="s">
         <v>122</v>
       </c>
@@ -3480,12 +3474,12 @@
         <v>124</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E30" s="2"/>
       <c r="F30" s="20"/>
       <c r="G30" s="4" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="H30" s="33">
         <v>28</v>
@@ -3494,7 +3488,7 @@
         <v>135</v>
       </c>
       <c r="J30" s="5" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="K30" s="66" t="s">
         <v>19</v>
@@ -3504,10 +3498,10 @@
       </c>
       <c r="M30" s="67"/>
       <c r="N30" s="14" t="s">
-        <v>275</v>
+        <v>267</v>
       </c>
       <c r="O30" s="20" t="s">
-        <v>266</v>
+        <v>258</v>
       </c>
       <c r="P30" s="21" t="s">
         <v>19</v>
@@ -3522,13 +3516,13 @@
         <v>129</v>
       </c>
       <c r="T30" s="8" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="U30" s="7" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="31" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="31" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="9" t="s">
         <v>122</v>
       </c>
@@ -3539,12 +3533,12 @@
         <v>124</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E31" s="2"/>
       <c r="F31" s="20"/>
       <c r="G31" s="4" t="s">
-        <v>228</v>
+        <v>271</v>
       </c>
       <c r="H31" s="33">
         <v>29</v>
@@ -3553,7 +3547,7 @@
         <v>135</v>
       </c>
       <c r="J31" s="5" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="K31" s="66" t="s">
         <v>19</v>
@@ -3563,31 +3557,31 @@
       </c>
       <c r="M31" s="67"/>
       <c r="N31" s="14" t="s">
-        <v>275</v>
+        <v>267</v>
       </c>
       <c r="O31" s="79" t="s">
-        <v>273</v>
+        <v>265</v>
       </c>
       <c r="P31" s="21" t="s">
         <v>19</v>
       </c>
       <c r="Q31" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="R31" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="R31" s="6" t="s">
-        <v>174</v>
-      </c>
       <c r="S31" s="7" t="s">
+        <v>222</v>
+      </c>
+      <c r="T31" s="8" t="s">
         <v>225</v>
       </c>
-      <c r="T31" s="8" t="s">
-        <v>229</v>
-      </c>
       <c r="U31" s="7" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="32" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="32" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="9" t="s">
         <v>122</v>
       </c>
@@ -3598,12 +3592,12 @@
         <v>124</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="E32" s="2"/>
       <c r="F32" s="20"/>
       <c r="G32" s="4" t="s">
-        <v>245</v>
+        <v>237</v>
       </c>
       <c r="H32" s="33">
         <v>30</v>
@@ -3612,7 +3606,7 @@
         <v>135</v>
       </c>
       <c r="J32" s="5" t="s">
-        <v>274</v>
+        <v>266</v>
       </c>
       <c r="K32" s="66" t="s">
         <v>20</v>
@@ -3632,7 +3626,7 @@
       <c r="T32" s="8"/>
       <c r="U32" s="7"/>
     </row>
-    <row r="33" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="33" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="9" t="s">
         <v>122</v>
       </c>
@@ -3643,12 +3637,12 @@
         <v>124</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="E33" s="2"/>
       <c r="F33" s="20"/>
       <c r="G33" s="4" t="s">
-        <v>246</v>
+        <v>238</v>
       </c>
       <c r="H33" s="33">
         <v>31</v>
@@ -3657,7 +3651,7 @@
         <v>135</v>
       </c>
       <c r="J33" s="5" t="s">
-        <v>276</v>
+        <v>268</v>
       </c>
       <c r="K33" s="66" t="s">
         <v>20</v>
@@ -3685,29 +3679,29 @@
         <v>138</v>
       </c>
       <c r="T33" s="8" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="U33" s="7" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="34" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="34" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" s="9" t="s">
         <v>122</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>240</v>
+        <v>123</v>
       </c>
       <c r="C34" s="11" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="E34" s="2"/>
       <c r="F34" s="20"/>
       <c r="G34" s="4" t="s">
-        <v>243</v>
+        <v>273</v>
       </c>
       <c r="H34" s="33">
         <v>32</v>
@@ -3716,7 +3710,7 @@
         <v>135</v>
       </c>
       <c r="J34" s="5" t="s">
-        <v>244</v>
+        <v>272</v>
       </c>
       <c r="K34" s="13" t="s">
         <v>19</v>
@@ -3732,13 +3726,23 @@
       <c r="P34" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="Q34" s="7"/>
-      <c r="R34" s="6"/>
-      <c r="S34" s="7"/>
-      <c r="T34" s="8"/>
-      <c r="U34" s="7"/>
-    </row>
-    <row r="35" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
+      <c r="Q34" s="7">
+        <v>6</v>
+      </c>
+      <c r="R34" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="S34" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="T34" s="8" t="s">
+        <v>274</v>
+      </c>
+      <c r="U34" s="7" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="35" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="9"/>
       <c r="B35" s="10"/>
       <c r="C35" s="11"/>
@@ -3761,7 +3765,7 @@
       <c r="T35" s="8"/>
       <c r="U35" s="7"/>
     </row>
-    <row r="36" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="36" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="9"/>
       <c r="B36" s="2"/>
       <c r="C36" s="3"/>
@@ -3784,7 +3788,7 @@
       <c r="T36" s="8"/>
       <c r="U36" s="7"/>
     </row>
-    <row r="37" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="37" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" s="9"/>
       <c r="B37" s="2"/>
       <c r="C37" s="3"/>
@@ -3807,7 +3811,7 @@
       <c r="T37" s="8"/>
       <c r="U37" s="7"/>
     </row>
-    <row r="38" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="38" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="9"/>
       <c r="B38" s="2"/>
       <c r="C38" s="3"/>
@@ -3830,7 +3834,7 @@
       <c r="T38" s="8"/>
       <c r="U38" s="7"/>
     </row>
-    <row r="39" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="39" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A39" s="9"/>
       <c r="B39" s="2"/>
       <c r="C39" s="3"/>
@@ -3853,7 +3857,7 @@
       <c r="T39" s="8"/>
       <c r="U39" s="7"/>
     </row>
-    <row r="40" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="40" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40" s="9"/>
       <c r="B40" s="2"/>
       <c r="C40" s="3"/>
@@ -3876,7 +3880,7 @@
       <c r="T40" s="8"/>
       <c r="U40" s="7"/>
     </row>
-    <row r="41" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="41" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41" s="9"/>
       <c r="B41" s="2"/>
       <c r="C41" s="3"/>
@@ -3899,7 +3903,7 @@
       <c r="T41" s="8"/>
       <c r="U41" s="7"/>
     </row>
-    <row r="42" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="42" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42" s="9"/>
       <c r="B42" s="2"/>
       <c r="C42" s="3"/>
@@ -3922,7 +3926,7 @@
       <c r="T42" s="8"/>
       <c r="U42" s="7"/>
     </row>
-    <row r="43" spans="1:21" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="43" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A43" s="9"/>
       <c r="B43" s="2"/>
       <c r="C43" s="3"/>
@@ -3945,187 +3949,187 @@
       <c r="T43" s="8"/>
       <c r="U43" s="7"/>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>117</v>
       </c>
@@ -4208,27 +4212,27 @@
       <selection activeCell="E52" sqref="E52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.3984375" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.86328125" style="23" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.3984375" style="23" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.86328125" style="23" customWidth="1"/>
+    <col min="1" max="1" width="21.85546875" style="23" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.42578125" style="23" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" style="23" customWidth="1"/>
     <col min="4" max="4" width="34" style="23" customWidth="1"/>
-    <col min="5" max="5" width="34.86328125" style="23" customWidth="1"/>
-    <col min="6" max="6" width="24.59765625" style="23" customWidth="1"/>
+    <col min="5" max="5" width="34.85546875" style="23" customWidth="1"/>
+    <col min="6" max="6" width="24.5703125" style="23" customWidth="1"/>
     <col min="7" max="7" width="18" style="23" customWidth="1"/>
-    <col min="8" max="8" width="12.73046875" style="23" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.86328125" style="23" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.73046875" style="23" customWidth="1"/>
-    <col min="11" max="11" width="15.59765625" style="23" customWidth="1"/>
+    <col min="8" max="8" width="12.7109375" style="23" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.85546875" style="23" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.7109375" style="23" customWidth="1"/>
+    <col min="11" max="11" width="15.5703125" style="23" customWidth="1"/>
     <col min="12" max="12" width="17" style="23" customWidth="1"/>
-    <col min="13" max="13" width="11.3984375" style="23"/>
-    <col min="14" max="14" width="24.265625" style="23" customWidth="1"/>
-    <col min="15" max="15" width="69.86328125" style="23" hidden="1" customWidth="1"/>
-    <col min="16" max="16384" width="11.3984375" style="23"/>
+    <col min="13" max="13" width="11.42578125" style="23"/>
+    <col min="14" max="14" width="24.28515625" style="23" customWidth="1"/>
+    <col min="15" max="15" width="69.85546875" style="23" hidden="1" customWidth="1"/>
+    <col min="16" max="16384" width="11.42578125" style="23"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="24" customFormat="1" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:12" s="24" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="23" t="s">
         <v>15</v>
       </c>
@@ -4245,7 +4249,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="23" t="s">
         <v>16</v>
       </c>
@@ -4269,7 +4273,7 @@
       <c r="K2" s="24"/>
       <c r="L2" s="24"/>
     </row>
-    <row r="3" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="23" t="s">
         <v>17</v>
       </c>
@@ -4288,7 +4292,7 @@
       <c r="K3" s="24"/>
       <c r="L3" s="24"/>
     </row>
-    <row r="4" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="23" t="s">
         <v>18</v>
       </c>
@@ -4307,7 +4311,7 @@
       <c r="K4" s="24"/>
       <c r="L4" s="24"/>
     </row>
-    <row r="5" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="23" t="s">
         <v>9</v>
       </c>
@@ -4323,7 +4327,7 @@
       <c r="K5" s="24"/>
       <c r="L5" s="24"/>
     </row>
-    <row r="6" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="23" t="s">
         <v>10</v>
       </c>
@@ -4340,7 +4344,7 @@
       <c r="K6" s="24"/>
       <c r="L6" s="24"/>
     </row>
-    <row r="7" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="23" t="s">
         <v>11</v>
       </c>
@@ -4357,7 +4361,7 @@
       <c r="K7" s="24"/>
       <c r="L7" s="24"/>
     </row>
-    <row r="8" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="24"/>
       <c r="C8" s="24"/>
       <c r="D8" s="24"/>
@@ -4372,7 +4376,7 @@
       <c r="K8" s="24"/>
       <c r="L8" s="24"/>
     </row>
-    <row r="9" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B9" s="24"/>
       <c r="C9" s="24"/>
       <c r="D9" s="24"/>
@@ -4387,7 +4391,7 @@
       <c r="K9" s="24"/>
       <c r="L9" s="24"/>
     </row>
-    <row r="10" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="24"/>
       <c r="C10" s="24"/>
       <c r="D10" s="24"/>
@@ -4402,7 +4406,7 @@
       <c r="K10" s="24"/>
       <c r="L10" s="24"/>
     </row>
-    <row r="11" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B11" s="24"/>
       <c r="C11" s="24"/>
       <c r="D11" s="24"/>
@@ -4417,7 +4421,7 @@
       <c r="K11" s="24"/>
       <c r="L11" s="24"/>
     </row>
-    <row r="12" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B12" s="24"/>
       <c r="C12" s="24"/>
       <c r="D12" s="24"/>
@@ -4432,7 +4436,7 @@
       <c r="K12" s="24"/>
       <c r="L12" s="24"/>
     </row>
-    <row r="13" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B13" s="24"/>
       <c r="C13" s="24"/>
       <c r="D13" s="24"/>
@@ -4447,7 +4451,7 @@
       <c r="K13" s="24"/>
       <c r="L13" s="24"/>
     </row>
-    <row r="14" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B14" s="24"/>
       <c r="C14" s="24"/>
       <c r="D14" s="24"/>
@@ -4462,7 +4466,7 @@
       <c r="K14" s="24"/>
       <c r="L14" s="24"/>
     </row>
-    <row r="15" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B15" s="24"/>
       <c r="C15" s="24"/>
       <c r="D15" s="24"/>
@@ -4477,7 +4481,7 @@
       <c r="K15" s="24"/>
       <c r="L15" s="24"/>
     </row>
-    <row r="16" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B16" s="24"/>
       <c r="C16" s="24"/>
       <c r="D16" s="24"/>
@@ -4492,7 +4496,7 @@
       <c r="K16" s="24"/>
       <c r="L16" s="24"/>
     </row>
-    <row r="17" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="17" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B17" s="24"/>
       <c r="D17" s="24"/>
       <c r="E17" s="23" t="s">
@@ -4506,7 +4510,7 @@
       <c r="K17" s="24"/>
       <c r="L17" s="24"/>
     </row>
-    <row r="18" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="18" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B18" s="24"/>
       <c r="D18" s="24"/>
       <c r="E18" s="23" t="s">
@@ -4520,7 +4524,7 @@
       <c r="K18" s="24"/>
       <c r="L18" s="24"/>
     </row>
-    <row r="19" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="19" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B19" s="24"/>
       <c r="D19" s="24"/>
       <c r="E19" s="23" t="s">
@@ -4534,7 +4538,7 @@
       <c r="K19" s="24"/>
       <c r="L19" s="24"/>
     </row>
-    <row r="20" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="20" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B20" s="24"/>
       <c r="D20" s="24"/>
       <c r="E20" s="23" t="s">
@@ -4548,7 +4552,7 @@
       <c r="K20" s="24"/>
       <c r="L20" s="24"/>
     </row>
-    <row r="21" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="21" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B21" s="24"/>
       <c r="C21" s="24"/>
       <c r="D21" s="24"/>
@@ -4563,7 +4567,7 @@
       <c r="K21" s="24"/>
       <c r="L21" s="24"/>
     </row>
-    <row r="22" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="22" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B22" s="24"/>
       <c r="C22" s="24"/>
       <c r="D22" s="24"/>
@@ -4578,7 +4582,7 @@
       <c r="K22" s="24"/>
       <c r="L22" s="24"/>
     </row>
-    <row r="23" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="23" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B23" s="24"/>
       <c r="C23" s="24"/>
       <c r="D23" s="24"/>
@@ -4593,7 +4597,7 @@
       <c r="K23" s="24"/>
       <c r="L23" s="24"/>
     </row>
-    <row r="24" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="24" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B24" s="24"/>
       <c r="C24" s="24"/>
       <c r="D24" s="24"/>
@@ -4608,7 +4612,7 @@
       <c r="K24" s="24"/>
       <c r="L24" s="24"/>
     </row>
-    <row r="25" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="25" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B25" s="24"/>
       <c r="C25" s="24"/>
       <c r="D25" s="24"/>
@@ -4623,7 +4627,7 @@
       <c r="K25" s="24"/>
       <c r="L25" s="24"/>
     </row>
-    <row r="26" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="26" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B26" s="24"/>
       <c r="C26" s="24"/>
       <c r="D26" s="24"/>
@@ -4638,7 +4642,7 @@
       <c r="K26" s="24"/>
       <c r="L26" s="24"/>
     </row>
-    <row r="27" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="27" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B27" s="24"/>
       <c r="C27" s="24"/>
       <c r="D27" s="24"/>
@@ -4653,7 +4657,7 @@
       <c r="K27" s="24"/>
       <c r="L27" s="24"/>
     </row>
-    <row r="28" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="28" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B28" s="24"/>
       <c r="C28" s="24"/>
       <c r="D28" s="24"/>
@@ -4668,7 +4672,7 @@
       <c r="K28" s="24"/>
       <c r="L28" s="24"/>
     </row>
-    <row r="29" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="29" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B29" s="24"/>
       <c r="C29" s="24"/>
       <c r="D29" s="24"/>
@@ -4683,7 +4687,7 @@
       <c r="K29" s="24"/>
       <c r="L29" s="24"/>
     </row>
-    <row r="30" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="30" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B30" s="24"/>
       <c r="C30" s="24"/>
       <c r="D30" s="24"/>
@@ -4698,7 +4702,7 @@
       <c r="K30" s="24"/>
       <c r="L30" s="24"/>
     </row>
-    <row r="31" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="31" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B31" s="24"/>
       <c r="C31" s="24"/>
       <c r="D31" s="24"/>
@@ -4713,7 +4717,7 @@
       <c r="K31" s="24"/>
       <c r="L31" s="24"/>
     </row>
-    <row r="32" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="32" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B32" s="24"/>
       <c r="C32" s="24"/>
       <c r="D32" s="24"/>
@@ -4728,7 +4732,7 @@
       <c r="K32" s="24"/>
       <c r="L32" s="24"/>
     </row>
-    <row r="33" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="33" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B33" s="24"/>
       <c r="C33" s="24"/>
       <c r="D33" s="24"/>
@@ -4743,7 +4747,7 @@
       <c r="K33" s="24"/>
       <c r="L33" s="24"/>
     </row>
-    <row r="34" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="34" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B34" s="24"/>
       <c r="C34" s="24"/>
       <c r="D34" s="24"/>
@@ -4758,7 +4762,7 @@
       <c r="K34" s="24"/>
       <c r="L34" s="24"/>
     </row>
-    <row r="35" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="35" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B35" s="24"/>
       <c r="C35" s="24"/>
       <c r="D35" s="24"/>
@@ -4773,7 +4777,7 @@
       <c r="K35" s="24"/>
       <c r="L35" s="24"/>
     </row>
-    <row r="36" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="36" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B36" s="24"/>
       <c r="C36" s="24"/>
       <c r="D36" s="24"/>
@@ -4788,7 +4792,7 @@
       <c r="K36" s="24"/>
       <c r="L36" s="24"/>
     </row>
-    <row r="37" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="37" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B37" s="24"/>
       <c r="C37" s="24"/>
       <c r="D37" s="24"/>
@@ -4803,7 +4807,7 @@
       <c r="K37" s="24"/>
       <c r="L37" s="24"/>
     </row>
-    <row r="38" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="38" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B38" s="24"/>
       <c r="C38" s="24"/>
       <c r="D38" s="24"/>
@@ -4818,7 +4822,7 @@
       <c r="K38" s="24"/>
       <c r="L38" s="24"/>
     </row>
-    <row r="39" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="39" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B39" s="24"/>
       <c r="C39" s="24"/>
       <c r="D39" s="24"/>
@@ -4833,7 +4837,7 @@
       <c r="K39" s="24"/>
       <c r="L39" s="24"/>
     </row>
-    <row r="40" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="40" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B40" s="24"/>
       <c r="C40" s="24"/>
       <c r="D40" s="24"/>
@@ -4848,7 +4852,7 @@
       <c r="K40" s="24"/>
       <c r="L40" s="24"/>
     </row>
-    <row r="41" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="41" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B41" s="24"/>
       <c r="C41" s="24"/>
       <c r="D41" s="24"/>
@@ -4863,7 +4867,7 @@
       <c r="K41" s="24"/>
       <c r="L41" s="24"/>
     </row>
-    <row r="42" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="42" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B42" s="24"/>
       <c r="C42" s="24"/>
       <c r="D42" s="24"/>
@@ -4878,7 +4882,7 @@
       <c r="K42" s="24"/>
       <c r="L42" s="24"/>
     </row>
-    <row r="43" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="43" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B43" s="24"/>
       <c r="C43" s="24"/>
       <c r="D43" s="24"/>
@@ -4893,7 +4897,7 @@
       <c r="K43" s="24"/>
       <c r="L43" s="24"/>
     </row>
-    <row r="44" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="44" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B44" s="24"/>
       <c r="C44" s="24"/>
       <c r="D44" s="24"/>
@@ -4908,7 +4912,7 @@
       <c r="K44" s="24"/>
       <c r="L44" s="24"/>
     </row>
-    <row r="45" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="45" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B45" s="24"/>
       <c r="C45" s="24"/>
       <c r="D45" s="24"/>
@@ -4923,7 +4927,7 @@
       <c r="K45" s="24"/>
       <c r="L45" s="24"/>
     </row>
-    <row r="46" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="46" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B46" s="24"/>
       <c r="C46" s="24"/>
       <c r="D46" s="24"/>
@@ -4938,7 +4942,7 @@
       <c r="K46" s="24"/>
       <c r="L46" s="24"/>
     </row>
-    <row r="47" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="47" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B47" s="24"/>
       <c r="C47" s="24"/>
       <c r="D47" s="24"/>
@@ -4953,7 +4957,7 @@
       <c r="K47" s="24"/>
       <c r="L47" s="24"/>
     </row>
-    <row r="48" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="48" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B48" s="24"/>
       <c r="C48" s="24"/>
       <c r="D48" s="24"/>
@@ -4968,7 +4972,7 @@
       <c r="K48" s="24"/>
       <c r="L48" s="24"/>
     </row>
-    <row r="49" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="49" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B49" s="24"/>
       <c r="C49" s="24"/>
       <c r="D49" s="24"/>
@@ -4980,7 +4984,7 @@
       <c r="K49" s="24"/>
       <c r="L49" s="24"/>
     </row>
-    <row r="50" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="50" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B50" s="24"/>
       <c r="C50" s="24"/>
       <c r="D50" s="24"/>
@@ -4992,7 +4996,7 @@
       <c r="K50" s="24"/>
       <c r="L50" s="24"/>
     </row>
-    <row r="51" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="51" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B51" s="24"/>
       <c r="C51" s="24"/>
       <c r="D51" s="24"/>
@@ -5005,7 +5009,7 @@
       <c r="K51" s="24"/>
       <c r="L51" s="24"/>
     </row>
-    <row r="52" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="52" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B52" s="24"/>
       <c r="C52" s="24"/>
       <c r="D52" s="24"/>
@@ -5018,7 +5022,7 @@
       <c r="K52" s="24"/>
       <c r="L52" s="24"/>
     </row>
-    <row r="53" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="53" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B53" s="24"/>
       <c r="C53" s="24"/>
       <c r="D53" s="24"/>
@@ -5031,7 +5035,7 @@
       <c r="K53" s="24"/>
       <c r="L53" s="24"/>
     </row>
-    <row r="54" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="54" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B54" s="24"/>
       <c r="C54" s="24"/>
       <c r="D54" s="24"/>
@@ -5044,7 +5048,7 @@
       <c r="K54" s="24"/>
       <c r="L54" s="24"/>
     </row>
-    <row r="55" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="55" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B55" s="24"/>
       <c r="C55" s="24"/>
       <c r="D55" s="24"/>
@@ -5057,7 +5061,7 @@
       <c r="K55" s="24"/>
       <c r="L55" s="24"/>
     </row>
-    <row r="56" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="56" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B56" s="24"/>
       <c r="C56" s="24"/>
       <c r="D56" s="24"/>
@@ -5070,7 +5074,7 @@
       <c r="K56" s="24"/>
       <c r="L56" s="24"/>
     </row>
-    <row r="57" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="57" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B57" s="24"/>
       <c r="C57" s="24"/>
       <c r="D57" s="24"/>
@@ -5083,7 +5087,7 @@
       <c r="K57" s="24"/>
       <c r="L57" s="24"/>
     </row>
-    <row r="58" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="58" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B58" s="24"/>
       <c r="C58" s="24"/>
       <c r="D58" s="24"/>
@@ -5096,7 +5100,7 @@
       <c r="K58" s="24"/>
       <c r="L58" s="24"/>
     </row>
-    <row r="59" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="59" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B59" s="24"/>
       <c r="C59" s="24"/>
       <c r="D59" s="24"/>
@@ -5109,7 +5113,7 @@
       <c r="K59" s="24"/>
       <c r="L59" s="24"/>
     </row>
-    <row r="60" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="60" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B60" s="24"/>
       <c r="C60" s="24"/>
       <c r="D60" s="24"/>
@@ -5122,7 +5126,7 @@
       <c r="K60" s="24"/>
       <c r="L60" s="24"/>
     </row>
-    <row r="61" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="61" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B61" s="24"/>
       <c r="C61" s="24"/>
       <c r="D61" s="24"/>
@@ -5135,7 +5139,7 @@
       <c r="K61" s="24"/>
       <c r="L61" s="24"/>
     </row>
-    <row r="62" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="62" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B62" s="24"/>
       <c r="C62" s="24"/>
       <c r="D62" s="24"/>
@@ -5148,7 +5152,7 @@
       <c r="K62" s="24"/>
       <c r="L62" s="24"/>
     </row>
-    <row r="63" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="63" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B63" s="24"/>
       <c r="C63" s="24"/>
       <c r="D63" s="24"/>
@@ -5161,7 +5165,7 @@
       <c r="K63" s="24"/>
       <c r="L63" s="24"/>
     </row>
-    <row r="64" spans="2:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="64" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B64" s="24"/>
       <c r="C64" s="24"/>
       <c r="D64" s="24"/>
@@ -5174,7 +5178,7 @@
       <c r="K64" s="24"/>
       <c r="L64" s="24"/>
     </row>
-    <row r="65" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="65" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B65" s="24"/>
       <c r="C65" s="24"/>
       <c r="D65" s="24"/>
@@ -5187,7 +5191,7 @@
       <c r="K65" s="24"/>
       <c r="L65" s="24"/>
     </row>
-    <row r="66" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="66" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B66" s="24"/>
       <c r="C66" s="24"/>
       <c r="D66" s="24"/>
@@ -5200,7 +5204,7 @@
       <c r="K66" s="24"/>
       <c r="L66" s="24"/>
     </row>
-    <row r="67" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="67" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B67" s="24"/>
       <c r="C67" s="24"/>
       <c r="D67" s="24"/>
@@ -5213,7 +5217,7 @@
       <c r="K67" s="24"/>
       <c r="L67" s="24"/>
     </row>
-    <row r="68" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="68" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B68" s="24"/>
       <c r="C68" s="24"/>
       <c r="D68" s="24"/>
@@ -5226,7 +5230,7 @@
       <c r="K68" s="24"/>
       <c r="L68" s="24"/>
     </row>
-    <row r="69" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="69" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B69" s="24"/>
       <c r="C69" s="24"/>
       <c r="D69" s="24"/>
@@ -5239,7 +5243,7 @@
       <c r="K69" s="24"/>
       <c r="L69" s="24"/>
     </row>
-    <row r="70" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="70" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B70" s="24"/>
       <c r="C70" s="24"/>
       <c r="D70" s="24"/>
@@ -5252,7 +5256,7 @@
       <c r="K70" s="24"/>
       <c r="L70" s="24"/>
     </row>
-    <row r="71" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="71" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A71" s="24"/>
       <c r="B71" s="24"/>
       <c r="C71" s="24"/>
@@ -5266,7 +5270,7 @@
       <c r="K71" s="24"/>
       <c r="L71" s="24"/>
     </row>
-    <row r="72" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="72" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A72" s="24"/>
       <c r="B72" s="24"/>
       <c r="C72" s="24"/>
@@ -5280,7 +5284,7 @@
       <c r="K72" s="24"/>
       <c r="L72" s="24"/>
     </row>
-    <row r="73" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="73" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A73" s="24"/>
       <c r="B73" s="24"/>
       <c r="C73" s="24"/>
@@ -5294,7 +5298,7 @@
       <c r="K73" s="24"/>
       <c r="L73" s="24"/>
     </row>
-    <row r="74" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="74" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A74" s="24"/>
       <c r="B74" s="24"/>
       <c r="C74" s="24"/>
@@ -5308,7 +5312,7 @@
       <c r="K74" s="24"/>
       <c r="L74" s="24"/>
     </row>
-    <row r="75" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="75" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A75" s="24"/>
       <c r="B75" s="24"/>
       <c r="C75" s="24"/>
@@ -5322,7 +5326,7 @@
       <c r="K75" s="24"/>
       <c r="L75" s="24"/>
     </row>
-    <row r="76" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="76" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A76" s="24"/>
       <c r="B76" s="24"/>
       <c r="C76" s="24"/>
@@ -5336,7 +5340,7 @@
       <c r="K76" s="24"/>
       <c r="L76" s="24"/>
     </row>
-    <row r="77" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="77" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A77" s="24"/>
       <c r="B77" s="24"/>
       <c r="C77" s="24"/>
@@ -5350,7 +5354,7 @@
       <c r="K77" s="24"/>
       <c r="L77" s="24"/>
     </row>
-    <row r="78" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="78" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A78" s="24"/>
       <c r="B78" s="24"/>
       <c r="C78" s="24"/>
@@ -5364,7 +5368,7 @@
       <c r="K78" s="24"/>
       <c r="L78" s="24"/>
     </row>
-    <row r="79" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="79" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A79" s="24"/>
       <c r="B79" s="24"/>
       <c r="C79" s="24"/>
@@ -5378,7 +5382,7 @@
       <c r="K79" s="24"/>
       <c r="L79" s="24"/>
     </row>
-    <row r="80" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="80" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A80" s="24"/>
       <c r="B80" s="24"/>
       <c r="C80" s="24"/>
@@ -5392,7 +5396,7 @@
       <c r="K80" s="24"/>
       <c r="L80" s="24"/>
     </row>
-    <row r="81" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="81" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A81" s="24"/>
       <c r="B81" s="24"/>
       <c r="C81" s="24"/>
@@ -5406,7 +5410,7 @@
       <c r="K81" s="24"/>
       <c r="L81" s="24"/>
     </row>
-    <row r="82" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="82" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A82" s="24"/>
       <c r="B82" s="24"/>
       <c r="C82" s="24"/>
@@ -5420,7 +5424,7 @@
       <c r="K82" s="24"/>
       <c r="L82" s="24"/>
     </row>
-    <row r="83" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="83" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A83" s="24"/>
       <c r="B83" s="24"/>
       <c r="C83" s="24"/>
@@ -5434,7 +5438,7 @@
       <c r="K83" s="24"/>
       <c r="L83" s="24"/>
     </row>
-    <row r="84" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="84" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A84" s="24"/>
       <c r="B84" s="24"/>
       <c r="C84" s="24"/>
@@ -5448,7 +5452,7 @@
       <c r="K84" s="24"/>
       <c r="L84" s="24"/>
     </row>
-    <row r="85" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="85" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A85" s="24"/>
       <c r="B85" s="24"/>
       <c r="C85" s="24"/>
@@ -5462,7 +5466,7 @@
       <c r="K85" s="24"/>
       <c r="L85" s="24"/>
     </row>
-    <row r="86" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="86" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A86" s="24"/>
       <c r="B86" s="24"/>
       <c r="C86" s="24"/>
@@ -5476,7 +5480,7 @@
       <c r="K86" s="24"/>
       <c r="L86" s="24"/>
     </row>
-    <row r="87" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="87" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A87" s="24"/>
       <c r="B87" s="24"/>
       <c r="C87" s="24"/>
@@ -5490,7 +5494,7 @@
       <c r="K87" s="24"/>
       <c r="L87" s="24"/>
     </row>
-    <row r="88" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="88" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A88" s="24"/>
       <c r="B88" s="24"/>
       <c r="C88" s="24"/>
@@ -5504,7 +5508,7 @@
       <c r="K88" s="24"/>
       <c r="L88" s="24"/>
     </row>
-    <row r="89" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="89" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A89" s="24"/>
       <c r="B89" s="24"/>
       <c r="C89" s="24"/>
@@ -5518,7 +5522,7 @@
       <c r="K89" s="24"/>
       <c r="L89" s="24"/>
     </row>
-    <row r="90" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="90" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A90" s="24"/>
       <c r="B90" s="24"/>
       <c r="C90" s="24"/>
@@ -5532,7 +5536,7 @@
       <c r="K90" s="24"/>
       <c r="L90" s="24"/>
     </row>
-    <row r="91" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="91" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A91" s="24"/>
       <c r="B91" s="24"/>
       <c r="C91" s="24"/>
@@ -5546,7 +5550,7 @@
       <c r="K91" s="24"/>
       <c r="L91" s="24"/>
     </row>
-    <row r="92" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="92" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A92" s="24"/>
       <c r="B92" s="24"/>
       <c r="C92" s="24"/>
@@ -5560,7 +5564,7 @@
       <c r="K92" s="24"/>
       <c r="L92" s="24"/>
     </row>
-    <row r="93" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="93" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A93" s="24"/>
       <c r="B93" s="24"/>
       <c r="C93" s="24"/>
@@ -5574,7 +5578,7 @@
       <c r="K93" s="24"/>
       <c r="L93" s="24"/>
     </row>
-    <row r="94" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="94" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A94" s="24"/>
       <c r="B94" s="24"/>
       <c r="C94" s="24"/>
@@ -5588,7 +5592,7 @@
       <c r="K94" s="24"/>
       <c r="L94" s="24"/>
     </row>
-    <row r="95" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="95" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A95" s="24"/>
       <c r="B95" s="24"/>
       <c r="C95" s="24"/>
@@ -5602,7 +5606,7 @@
       <c r="K95" s="24"/>
       <c r="L95" s="24"/>
     </row>
-    <row r="96" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="96" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A96" s="24"/>
       <c r="B96" s="24"/>
       <c r="C96" s="24"/>
@@ -5616,7 +5620,7 @@
       <c r="K96" s="24"/>
       <c r="L96" s="24"/>
     </row>
-    <row r="97" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="97" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A97" s="24"/>
       <c r="B97" s="24"/>
       <c r="C97" s="24"/>
@@ -5630,7 +5634,7 @@
       <c r="K97" s="24"/>
       <c r="L97" s="24"/>
     </row>
-    <row r="98" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="98" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A98" s="24"/>
       <c r="B98" s="24"/>
       <c r="C98" s="24"/>
@@ -5644,7 +5648,7 @@
       <c r="K98" s="24"/>
       <c r="L98" s="24"/>
     </row>
-    <row r="99" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="99" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A99" s="24"/>
       <c r="B99" s="24"/>
       <c r="C99" s="24"/>
@@ -5658,7 +5662,7 @@
       <c r="K99" s="24"/>
       <c r="L99" s="24"/>
     </row>
-    <row r="100" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="100" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A100" s="24"/>
       <c r="B100" s="24"/>
       <c r="C100" s="24"/>
@@ -5672,7 +5676,7 @@
       <c r="K100" s="24"/>
       <c r="L100" s="24"/>
     </row>
-    <row r="101" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="101" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A101" s="24"/>
       <c r="B101" s="24"/>
       <c r="C101" s="24"/>
@@ -5686,7 +5690,7 @@
       <c r="K101" s="24"/>
       <c r="L101" s="24"/>
     </row>
-    <row r="102" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="102" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A102" s="24"/>
       <c r="B102" s="24"/>
       <c r="C102" s="24"/>
@@ -5700,7 +5704,7 @@
       <c r="K102" s="24"/>
       <c r="L102" s="24"/>
     </row>
-    <row r="103" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="103" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A103" s="24"/>
       <c r="B103" s="24"/>
       <c r="C103" s="24"/>
@@ -5714,7 +5718,7 @@
       <c r="K103" s="24"/>
       <c r="L103" s="24"/>
     </row>
-    <row r="104" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="104" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A104" s="24"/>
       <c r="B104" s="24"/>
       <c r="C104" s="24"/>
@@ -5728,7 +5732,7 @@
       <c r="K104" s="24"/>
       <c r="L104" s="24"/>
     </row>
-    <row r="105" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="105" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A105" s="24"/>
       <c r="B105" s="24"/>
       <c r="C105" s="24"/>
@@ -5742,7 +5746,7 @@
       <c r="K105" s="24"/>
       <c r="L105" s="24"/>
     </row>
-    <row r="106" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="106" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A106" s="24"/>
       <c r="B106" s="24"/>
       <c r="C106" s="24"/>
@@ -5756,7 +5760,7 @@
       <c r="K106" s="24"/>
       <c r="L106" s="24"/>
     </row>
-    <row r="107" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="107" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A107" s="24"/>
       <c r="B107" s="24"/>
       <c r="C107" s="24"/>
@@ -5770,7 +5774,7 @@
       <c r="K107" s="24"/>
       <c r="L107" s="24"/>
     </row>
-    <row r="108" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="108" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A108" s="24"/>
       <c r="B108" s="24"/>
       <c r="C108" s="24"/>
@@ -5784,7 +5788,7 @@
       <c r="K108" s="24"/>
       <c r="L108" s="24"/>
     </row>
-    <row r="109" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="109" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A109" s="24"/>
       <c r="B109" s="24"/>
       <c r="C109" s="24"/>
@@ -5798,7 +5802,7 @@
       <c r="K109" s="24"/>
       <c r="L109" s="24"/>
     </row>
-    <row r="110" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="110" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A110" s="24"/>
       <c r="B110" s="24"/>
       <c r="C110" s="24"/>
@@ -5812,7 +5816,7 @@
       <c r="K110" s="24"/>
       <c r="L110" s="24"/>
     </row>
-    <row r="111" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="111" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A111" s="24"/>
       <c r="B111" s="24"/>
       <c r="C111" s="24"/>
@@ -5826,7 +5830,7 @@
       <c r="K111" s="24"/>
       <c r="L111" s="24"/>
     </row>
-    <row r="112" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="112" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A112" s="24"/>
       <c r="B112" s="24"/>
       <c r="C112" s="24"/>
@@ -5840,7 +5844,7 @@
       <c r="K112" s="24"/>
       <c r="L112" s="24"/>
     </row>
-    <row r="113" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="113" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A113" s="24"/>
       <c r="B113" s="24"/>
       <c r="C113" s="24"/>
@@ -5854,7 +5858,7 @@
       <c r="K113" s="24"/>
       <c r="L113" s="24"/>
     </row>
-    <row r="114" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="114" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A114" s="24"/>
       <c r="B114" s="24"/>
       <c r="C114" s="24"/>
@@ -5868,7 +5872,7 @@
       <c r="K114" s="24"/>
       <c r="L114" s="24"/>
     </row>
-    <row r="115" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="115" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A115" s="24"/>
       <c r="B115" s="24"/>
       <c r="C115" s="24"/>
@@ -5882,7 +5886,7 @@
       <c r="K115" s="24"/>
       <c r="L115" s="24"/>
     </row>
-    <row r="116" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="116" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A116" s="24"/>
       <c r="B116" s="24"/>
       <c r="C116" s="24"/>
@@ -5896,7 +5900,7 @@
       <c r="K116" s="24"/>
       <c r="L116" s="24"/>
     </row>
-    <row r="117" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="117" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A117" s="24"/>
       <c r="B117" s="24"/>
       <c r="C117" s="24"/>
@@ -5910,7 +5914,7 @@
       <c r="K117" s="24"/>
       <c r="L117" s="24"/>
     </row>
-    <row r="118" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="118" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A118" s="24"/>
       <c r="B118" s="24"/>
       <c r="C118" s="24"/>
@@ -5924,7 +5928,7 @@
       <c r="K118" s="24"/>
       <c r="L118" s="24"/>
     </row>
-    <row r="119" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="119" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A119" s="24"/>
       <c r="B119" s="24"/>
       <c r="C119" s="24"/>
@@ -5938,7 +5942,7 @@
       <c r="K119" s="24"/>
       <c r="L119" s="24"/>
     </row>
-    <row r="120" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="120" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A120" s="24"/>
       <c r="B120" s="24"/>
       <c r="C120" s="24"/>
@@ -5952,7 +5956,7 @@
       <c r="K120" s="24"/>
       <c r="L120" s="24"/>
     </row>
-    <row r="121" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="121" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A121" s="24"/>
       <c r="B121" s="24"/>
       <c r="C121" s="24"/>
@@ -5966,7 +5970,7 @@
       <c r="K121" s="24"/>
       <c r="L121" s="24"/>
     </row>
-    <row r="122" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="122" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A122" s="24"/>
       <c r="B122" s="24"/>
       <c r="C122" s="24"/>
@@ -5980,7 +5984,7 @@
       <c r="K122" s="24"/>
       <c r="L122" s="24"/>
     </row>
-    <row r="123" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="123" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A123" s="24"/>
       <c r="B123" s="24"/>
       <c r="C123" s="24"/>
@@ -5994,7 +5998,7 @@
       <c r="K123" s="24"/>
       <c r="L123" s="24"/>
     </row>
-    <row r="124" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="124" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A124" s="24"/>
       <c r="B124" s="24"/>
       <c r="C124" s="24"/>
@@ -6008,7 +6012,7 @@
       <c r="K124" s="24"/>
       <c r="L124" s="24"/>
     </row>
-    <row r="125" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="125" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A125" s="24"/>
       <c r="B125" s="24"/>
       <c r="C125" s="24"/>
@@ -6022,7 +6026,7 @@
       <c r="K125" s="24"/>
       <c r="L125" s="24"/>
     </row>
-    <row r="126" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="126" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A126" s="24"/>
       <c r="B126" s="24"/>
       <c r="C126" s="24"/>
@@ -6036,7 +6040,7 @@
       <c r="K126" s="24"/>
       <c r="L126" s="24"/>
     </row>
-    <row r="127" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="127" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A127" s="24"/>
       <c r="B127" s="24"/>
       <c r="C127" s="24"/>
@@ -6050,7 +6054,7 @@
       <c r="K127" s="24"/>
       <c r="L127" s="24"/>
     </row>
-    <row r="128" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="128" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A128" s="24"/>
       <c r="B128" s="24"/>
       <c r="C128" s="24"/>
@@ -6064,7 +6068,7 @@
       <c r="K128" s="24"/>
       <c r="L128" s="24"/>
     </row>
-    <row r="129" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="129" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A129" s="24"/>
       <c r="B129" s="24"/>
       <c r="C129" s="24"/>
@@ -6078,7 +6082,7 @@
       <c r="K129" s="24"/>
       <c r="L129" s="24"/>
     </row>
-    <row r="130" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="130" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A130" s="24"/>
       <c r="B130" s="24"/>
       <c r="C130" s="24"/>
@@ -6092,7 +6096,7 @@
       <c r="K130" s="24"/>
       <c r="L130" s="24"/>
     </row>
-    <row r="131" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="131" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A131" s="24"/>
       <c r="B131" s="24"/>
       <c r="C131" s="24"/>
@@ -6106,7 +6110,7 @@
       <c r="K131" s="24"/>
       <c r="L131" s="24"/>
     </row>
-    <row r="132" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="132" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A132" s="24"/>
       <c r="B132" s="24"/>
       <c r="C132" s="24"/>
@@ -6120,7 +6124,7 @@
       <c r="K132" s="24"/>
       <c r="L132" s="24"/>
     </row>
-    <row r="133" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
+    <row r="133" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A133" s="24"/>
       <c r="B133" s="24"/>
       <c r="C133" s="24"/>

</xml_diff>